<commit_message>
Actualizado el item 5 con la version final del proyecto
</commit_message>
<xml_diff>
--- a/Item 1/CostesDP.xlsx
+++ b/Item 1/CostesDP.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17766"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17830"/>
   <workbookPr filterPrivacy="1"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
@@ -378,10 +378,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I8"/>
+  <dimension ref="A1:I16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -427,7 +427,7 @@
         <v>6</v>
       </c>
       <c r="B2">
-        <v>40.01</v>
+        <v>16.78</v>
       </c>
       <c r="C2">
         <v>1000</v>
@@ -439,19 +439,19 @@
         <v>0</v>
       </c>
       <c r="F2">
-        <v>22</v>
+        <v>14</v>
       </c>
       <c r="G2">
-        <f>B2*F2+(((B2+E2)/5760)*C2)+D2</f>
-        <v>1038.6061805555555</v>
+        <f>B2*F2+(((B2+E2)/5760)*C2)+D2/8/4*3</f>
+        <v>252.03069444444446</v>
       </c>
       <c r="H2">
         <f>((B2)/5760)*C2</f>
-        <v>6.9461805555555554</v>
+        <v>2.9131944444444446</v>
       </c>
       <c r="I2">
         <f>B2*F2</f>
-        <v>880.21999999999991</v>
+        <v>234.92000000000002</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
@@ -459,7 +459,7 @@
         <v>7</v>
       </c>
       <c r="B3">
-        <v>63</v>
+        <v>22.43</v>
       </c>
       <c r="C3">
         <v>800</v>
@@ -474,16 +474,16 @@
         <v>14</v>
       </c>
       <c r="G3">
-        <f t="shared" ref="G3:G7" si="0">B3*F3+(((B3+E3)/5760)*C3)+D3</f>
-        <v>1042.19</v>
+        <f>B3*F3+(((B3+E3)/5760)*C3)+D3/8/4*3</f>
+        <v>331.33277777777778</v>
       </c>
       <c r="H3">
-        <f t="shared" ref="H3:H7" si="1">((B3)/5760)*C3</f>
-        <v>8.75</v>
+        <f t="shared" ref="H3:H7" si="0">((B3)/5760)*C3</f>
+        <v>3.1152777777777776</v>
       </c>
       <c r="I3">
-        <f t="shared" ref="I3:I7" si="2">B3*F3</f>
-        <v>882</v>
+        <f t="shared" ref="I3:I7" si="1">B3*F3</f>
+        <v>314.02</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
@@ -491,7 +491,7 @@
         <v>0</v>
       </c>
       <c r="B4">
-        <v>64.599999999999994</v>
+        <v>19.53</v>
       </c>
       <c r="C4">
         <v>850</v>
@@ -506,16 +506,16 @@
         <v>14</v>
       </c>
       <c r="G4">
+        <f>B4*F4+(((B4+E4)/5760)*C4)+D4/8/4*3</f>
+        <v>290.49953125000002</v>
+      </c>
+      <c r="H4">
         <f t="shared" si="0"/>
-        <v>1065.372986111111</v>
-      </c>
-      <c r="H4">
+        <v>2.8820312500000003</v>
+      </c>
+      <c r="I4">
         <f t="shared" si="1"/>
-        <v>9.5329861111111107</v>
-      </c>
-      <c r="I4">
-        <f t="shared" si="2"/>
-        <v>904.39999999999986</v>
+        <v>273.42</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
@@ -523,7 +523,7 @@
         <v>8</v>
       </c>
       <c r="B5">
-        <v>42.75</v>
+        <v>28.23</v>
       </c>
       <c r="C5">
         <v>750</v>
@@ -538,16 +538,16 @@
         <v>14</v>
       </c>
       <c r="G5">
+        <f>B5*F5+(((B5+E5)/5760)*C5)+D5/8/4*3</f>
+        <v>413.09328125000002</v>
+      </c>
+      <c r="H5">
         <f t="shared" si="0"/>
-        <v>755.50640625000005</v>
-      </c>
-      <c r="H5">
+        <v>3.67578125</v>
+      </c>
+      <c r="I5">
         <f t="shared" si="1"/>
-        <v>5.56640625</v>
-      </c>
-      <c r="I5">
-        <f t="shared" si="2"/>
-        <v>598.5</v>
+        <v>395.22</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
@@ -555,7 +555,7 @@
         <v>9</v>
       </c>
       <c r="B6">
-        <v>55.95</v>
+        <v>36.68</v>
       </c>
       <c r="C6">
         <v>1200</v>
@@ -567,19 +567,19 @@
         <v>0</v>
       </c>
       <c r="F6">
-        <v>14</v>
+        <v>22</v>
       </c>
       <c r="G6">
+        <f>B6*F6+(((B6+E6)/5760)*C6)+D6/8/4*3</f>
+        <v>828.79916666666668</v>
+      </c>
+      <c r="H6">
         <f t="shared" si="0"/>
-        <v>946.39625000000001</v>
-      </c>
-      <c r="H6">
+        <v>7.6416666666666666</v>
+      </c>
+      <c r="I6">
         <f t="shared" si="1"/>
-        <v>11.65625</v>
-      </c>
-      <c r="I6">
-        <f t="shared" si="2"/>
-        <v>783.30000000000007</v>
+        <v>806.96</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
@@ -587,7 +587,7 @@
         <v>10</v>
       </c>
       <c r="B7">
-        <v>40.5</v>
+        <v>18.98</v>
       </c>
       <c r="C7">
         <v>1400</v>
@@ -602,22 +602,22 @@
         <v>14</v>
       </c>
       <c r="G7">
+        <f>B7*F7+(((B7+E7)/5760)*C7)+D7/8/4*3</f>
+        <v>284.53069444444446</v>
+      </c>
+      <c r="H7">
         <f t="shared" si="0"/>
-        <v>728.28375000000005</v>
-      </c>
-      <c r="H7">
+        <v>4.6131944444444448</v>
+      </c>
+      <c r="I7">
         <f t="shared" si="1"/>
-        <v>9.84375</v>
-      </c>
-      <c r="I7">
-        <f t="shared" si="2"/>
-        <v>567</v>
+        <v>265.72000000000003</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B8">
         <f>SUM(B2:B7)</f>
-        <v>306.81</v>
+        <v>142.63</v>
       </c>
       <c r="D8">
         <f>SUM(D2:D7)</f>
@@ -625,15 +625,33 @@
       </c>
       <c r="G8">
         <f>SUM(G2:G7)</f>
-        <v>5576.3555729166674</v>
+        <v>2400.2861458333336</v>
       </c>
       <c r="H8">
-        <f t="shared" ref="H8:I8" si="3">SUM(H2:H7)</f>
-        <v>52.295572916666664</v>
+        <f t="shared" ref="H8:I8" si="2">SUM(H2:H7)</f>
+        <v>24.841145833333336</v>
       </c>
       <c r="I8">
-        <f t="shared" si="3"/>
-        <v>4615.42</v>
+        <f t="shared" si="2"/>
+        <v>2290.2600000000002</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="F14">
+        <f>151.44/8/4*3*6</f>
+        <v>85.185000000000002</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B15">
+        <f>B2+B3+B4+B5+B7</f>
+        <v>105.95</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C16">
+        <f>B15+B6</f>
+        <v>142.63</v>
       </c>
     </row>
   </sheetData>

</xml_diff>